<commit_message>
Initial commit: Add Node.js project setup
</commit_message>
<xml_diff>
--- a/public/assets/receipts.xlsx
+++ b/public/assets/receipts.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" rightToLeft="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -448,86 +448,45 @@
         <v>00001</v>
       </c>
       <c r="B2" t="str">
-        <v>Rhanyra Targaryan</v>
+        <v>Jibin Roy</v>
       </c>
       <c r="C2" t="str">
-        <v>8976540123</v>
+        <v>8111849588</v>
       </c>
       <c r="D2" t="str">
-        <v>rhanyra.targaryan@gmail.com</v>
+        <v>jibinroy949@gmail.com</v>
       </c>
       <c r="E2" t="str">
-        <v>Dracarys</v>
+        <v>qwerty</v>
       </c>
       <c r="F2" t="str">
-        <v>Jun-2024</v>
+        <v>Aug-2024</v>
       </c>
       <c r="G2" t="str">
-        <v>Double Private</v>
+        <v>Single Private</v>
       </c>
       <c r="H2" t="str">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="str">
-        <v>24998</v>
+        <v>15000</v>
       </c>
       <c r="J2" t="str">
-        <v>Deposit</v>
+        <v>Monthly Rent</v>
       </c>
       <c r="K2" t="str">
-        <v>Cash</v>
+        <v>UPI</v>
       </c>
       <c r="L2" t="str">
         <v>Paid</v>
       </c>
       <c r="M2" t="str">
-        <v>07-12-2024</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>00002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Dean Winchestor</v>
-      </c>
-      <c r="C3" t="str">
-        <v>8791450236</v>
-      </c>
-      <c r="D3" t="str">
-        <v>dean.winchestor@gmail.com</v>
-      </c>
-      <c r="E3" t="str">
-        <v>demonhunter</v>
-      </c>
-      <c r="F3" t="str">
-        <v>Apr-2024</v>
-      </c>
-      <c r="G3" t="str">
-        <v>Single Private</v>
-      </c>
-      <c r="H3" t="str">
-        <v>1</v>
-      </c>
-      <c r="I3" t="str">
-        <v>15000</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Monthly Rent</v>
-      </c>
-      <c r="K3" t="str">
-        <v>Credit Card</v>
-      </c>
-      <c r="L3" t="str">
-        <v>Paid</v>
-      </c>
-      <c r="M3" t="str">
         <v>07-12-2024</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>